<commit_message>
fixed player mover, added slider to rotate platform
</commit_message>
<xml_diff>
--- a/ImportedItems.xlsx
+++ b/ImportedItems.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1716A4B-AC3B-4AE2-B47E-99B1151865A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769C79B4-65A3-4593-901E-E5DA0DB55199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>what</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Assets/AurynSky</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>https://free3d.com/3d-model/coin-4532.html</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,10 +485,19 @@
         <v>4</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{19A89ED8-EC70-4C9F-B428-4A56FE1A4C4F}"/>
     <hyperlink ref="D3" r:id="rId2" location="content" xr:uid="{D406BF71-EEE2-4E23-9556-AFC278B6832F}"/>
+    <hyperlink ref="D11" r:id="rId3" xr:uid="{7605F01A-1296-4D7C-A9C8-761046F4EE5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new characters changed states script
</commit_message>
<xml_diff>
--- a/ImportedItems.xlsx
+++ b/ImportedItems.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769C79B4-65A3-4593-901E-E5DA0DB55199}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FA1C8D-4A8C-4B88-8B72-778E2714BA81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>what</t>
   </si>
@@ -38,18 +38,6 @@
   </si>
   <si>
     <t>Assets</t>
-  </si>
-  <si>
-    <t>https://assetstore.unity.com/packages/3d/characters/animals/toon-fox-183005#content</t>
-  </si>
-  <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>Assets/Fox</t>
-  </si>
-  <si>
-    <t>player</t>
   </si>
   <si>
     <t>https://assetstore.unity.com/packages/3d/props/simple-gems-ultimate-animated-customizable-pack-73764</t>
@@ -418,7 +406,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C5" sqref="C5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,18 +436,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -471,14 +449,17 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -487,17 +468,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{19A89ED8-EC70-4C9F-B428-4A56FE1A4C4F}"/>
-    <hyperlink ref="D3" r:id="rId2" location="content" xr:uid="{D406BF71-EEE2-4E23-9556-AFC278B6832F}"/>
-    <hyperlink ref="D11" r:id="rId3" xr:uid="{7605F01A-1296-4D7C-A9C8-761046F4EE5A}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{7605F01A-1296-4D7C-A9C8-761046F4EE5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>